<commit_message>
User sign up page created
</commit_message>
<xml_diff>
--- a/excel layout/Survivor Start.xlsx
+++ b/excel layout/Survivor Start.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thoma\Work_application_folder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thoma\Work_application_folder\survivor_game2\survivor_game\excel layout\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE2BC9E0-4F26-4737-9880-122768DA8D8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6B41FC7-1F71-4370-9E48-B3FD64A95BB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{01AAC2B4-48A1-4B4E-9AE4-9846F6EC1D84}"/>
   </bookViews>
@@ -630,7 +630,7 @@
   <dimension ref="A1:V26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -723,7 +723,7 @@
         <v>27</v>
       </c>
       <c r="Q2">
-        <v>4.9050331115722656E-2</v>
+        <v>17.850383758544922</v>
       </c>
       <c r="R2">
         <v>0</v>
@@ -747,53 +747,57 @@
       </c>
       <c r="B3" s="2">
         <f ca="1">IFERROR(1 + (13.28771237 * LOG(1 + (O3/$B$26))), 1)</f>
-        <v>1.31847151062889</v>
+        <v>1.2595583471732017</v>
       </c>
       <c r="C3">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D3">
         <f ca="1">IFERROR(C3*B3, 0)</f>
-        <v>6.59235755314445</v>
+        <v>0</v>
       </c>
       <c r="E3">
         <v>5</v>
       </c>
       <c r="F3">
         <f ca="1">IFERROR(E3*B3, 0)</f>
-        <v>6.59235755314445</v>
+        <v>6.2977917358660083</v>
       </c>
       <c r="G3">
         <v>5</v>
       </c>
       <c r="H3">
         <f t="shared" ref="H3:H20" ca="1" si="0">IFERROR(G3*B3, 0)</f>
-        <v>6.59235755314445</v>
+        <v>6.2977917358660083</v>
       </c>
       <c r="I3">
         <v>5</v>
       </c>
       <c r="J3">
         <f ca="1">IFERROR(I3*B3, 0)</f>
-        <v>6.59235755314445</v>
+        <v>6.2977917358660083</v>
       </c>
       <c r="K3">
         <v>5</v>
       </c>
       <c r="L3">
         <f ca="1">IFERROR(K3*B3, 0)</f>
-        <v>6.59235755314445</v>
+        <v>6.2977917358660083</v>
       </c>
       <c r="M3">
         <v>5</v>
       </c>
       <c r="N3">
         <f ca="1">IFERROR(M3*B3, 0)</f>
-        <v>6.59235755314445</v>
+        <v>6.2977917358660083</v>
       </c>
       <c r="O3">
         <f t="shared" ref="O3:O20" ca="1" si="1">D3+F3+H3+J3+L3+N3</f>
-        <v>39.554145318866702</v>
+        <v>31.48895867933004</v>
+      </c>
+      <c r="Q3">
+        <f ca="1">D21+Q2</f>
+        <v>111.94294203941153</v>
       </c>
     </row>
     <row r="4" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -802,53 +806,53 @@
       </c>
       <c r="B4" s="2">
         <f t="shared" ref="B4:B20" ca="1" si="2">IFERROR(1 + (13.28771237 * LOG(1 + (O4/$B$26))), 1)</f>
-        <v>1.31847151062889</v>
+        <v>1.2595583471732017</v>
       </c>
       <c r="C4">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D4">
         <f t="shared" ref="D4:D20" ca="1" si="3">IFERROR(C4*B4, 0)</f>
-        <v>6.59235755314445</v>
+        <v>0</v>
       </c>
       <c r="E4">
         <v>5</v>
       </c>
       <c r="F4">
         <f t="shared" ref="F4:F20" ca="1" si="4">IFERROR(E4*B4, 0)</f>
-        <v>6.59235755314445</v>
+        <v>6.2977917358660083</v>
       </c>
       <c r="G4">
         <v>5</v>
       </c>
       <c r="H4">
         <f t="shared" ca="1" si="0"/>
-        <v>6.59235755314445</v>
+        <v>6.2977917358660083</v>
       </c>
       <c r="I4">
         <v>5</v>
       </c>
       <c r="J4">
         <f t="shared" ref="J4:J20" ca="1" si="5">IFERROR(I4*B4, 0)</f>
-        <v>6.59235755314445</v>
+        <v>6.2977917358660083</v>
       </c>
       <c r="K4">
         <v>5</v>
       </c>
       <c r="L4">
         <f t="shared" ref="L4:L20" ca="1" si="6">IFERROR(K4*B4, 0)</f>
-        <v>6.59235755314445</v>
+        <v>6.2977917358660083</v>
       </c>
       <c r="M4">
         <v>5</v>
       </c>
       <c r="N4">
         <f t="shared" ref="N4:N20" ca="1" si="7">IFERROR(M4*B4, 0)</f>
-        <v>6.59235755314445</v>
+        <v>6.2977917358660083</v>
       </c>
       <c r="O4">
         <f t="shared" ca="1" si="1"/>
-        <v>39.554145318866702</v>
+        <v>31.48895867933004</v>
       </c>
     </row>
     <row r="5" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -857,53 +861,53 @@
       </c>
       <c r="B5" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>1.31847151062889</v>
+        <v>1.3260025079320772</v>
       </c>
       <c r="C5">
         <v>5</v>
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="3"/>
-        <v>6.59235755314445</v>
+        <v>6.6300125396603864</v>
       </c>
       <c r="E5">
         <v>5</v>
       </c>
       <c r="F5">
         <f t="shared" ca="1" si="4"/>
-        <v>6.59235755314445</v>
+        <v>6.6300125396603864</v>
       </c>
       <c r="G5">
         <v>5</v>
       </c>
       <c r="H5">
         <f t="shared" ca="1" si="0"/>
-        <v>6.59235755314445</v>
+        <v>6.6300125396603864</v>
       </c>
       <c r="I5">
         <v>5</v>
       </c>
       <c r="J5">
         <f t="shared" ca="1" si="5"/>
-        <v>6.59235755314445</v>
+        <v>6.6300125396603864</v>
       </c>
       <c r="K5">
         <v>5</v>
       </c>
       <c r="L5">
         <f t="shared" ca="1" si="6"/>
-        <v>6.59235755314445</v>
+        <v>6.6300125396603864</v>
       </c>
       <c r="M5">
         <v>5</v>
       </c>
       <c r="N5">
         <f t="shared" ca="1" si="7"/>
-        <v>6.59235755314445</v>
+        <v>6.6300125396603864</v>
       </c>
       <c r="O5">
         <f t="shared" ca="1" si="1"/>
-        <v>39.554145318866702</v>
+        <v>39.780075237962315</v>
       </c>
     </row>
     <row r="6" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -912,53 +916,53 @@
       </c>
       <c r="B6" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>1.31847151062889</v>
+        <v>1.3260025079320772</v>
       </c>
       <c r="C6">
         <v>5</v>
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="3"/>
-        <v>6.59235755314445</v>
+        <v>6.6300125396603864</v>
       </c>
       <c r="E6">
         <v>5</v>
       </c>
       <c r="F6">
         <f t="shared" ca="1" si="4"/>
-        <v>6.59235755314445</v>
+        <v>6.6300125396603864</v>
       </c>
       <c r="G6">
         <v>5</v>
       </c>
       <c r="H6">
         <f t="shared" ca="1" si="0"/>
-        <v>6.59235755314445</v>
+        <v>6.6300125396603864</v>
       </c>
       <c r="I6">
         <v>5</v>
       </c>
       <c r="J6">
         <f t="shared" ca="1" si="5"/>
-        <v>6.59235755314445</v>
+        <v>6.6300125396603864</v>
       </c>
       <c r="K6">
         <v>5</v>
       </c>
       <c r="L6">
         <f t="shared" ca="1" si="6"/>
-        <v>6.59235755314445</v>
+        <v>6.6300125396603864</v>
       </c>
       <c r="M6">
         <v>5</v>
       </c>
       <c r="N6">
         <f t="shared" ca="1" si="7"/>
-        <v>6.59235755314445</v>
+        <v>6.6300125396603864</v>
       </c>
       <c r="O6">
         <f t="shared" ca="1" si="1"/>
-        <v>39.554145318866702</v>
+        <v>39.780075237962315</v>
       </c>
     </row>
     <row r="7" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -967,53 +971,53 @@
       </c>
       <c r="B7" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>1.31847151062889</v>
+        <v>1.3260025079320772</v>
       </c>
       <c r="C7">
         <v>5</v>
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="3"/>
-        <v>6.59235755314445</v>
+        <v>6.6300125396603864</v>
       </c>
       <c r="E7">
         <v>5</v>
       </c>
       <c r="F7">
         <f t="shared" ca="1" si="4"/>
-        <v>6.59235755314445</v>
+        <v>6.6300125396603864</v>
       </c>
       <c r="G7">
         <v>5</v>
       </c>
       <c r="H7">
         <f t="shared" ca="1" si="0"/>
-        <v>6.59235755314445</v>
+        <v>6.6300125396603864</v>
       </c>
       <c r="I7">
         <v>5</v>
       </c>
       <c r="J7">
         <f t="shared" ca="1" si="5"/>
-        <v>6.59235755314445</v>
+        <v>6.6300125396603864</v>
       </c>
       <c r="K7">
         <v>5</v>
       </c>
       <c r="L7">
         <f t="shared" ca="1" si="6"/>
-        <v>6.59235755314445</v>
+        <v>6.6300125396603864</v>
       </c>
       <c r="M7">
         <v>5</v>
       </c>
       <c r="N7">
         <f t="shared" ca="1" si="7"/>
-        <v>6.59235755314445</v>
+        <v>6.6300125396603864</v>
       </c>
       <c r="O7">
         <f t="shared" ca="1" si="1"/>
-        <v>39.554145318866702</v>
+        <v>39.780075237962315</v>
       </c>
     </row>
     <row r="8" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1022,53 +1026,53 @@
       </c>
       <c r="B8" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>1.31847151062889</v>
+        <v>1.3260025079320772</v>
       </c>
       <c r="C8">
         <v>5</v>
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="3"/>
-        <v>6.59235755314445</v>
+        <v>6.6300125396603864</v>
       </c>
       <c r="E8">
         <v>5</v>
       </c>
       <c r="F8">
         <f t="shared" ca="1" si="4"/>
-        <v>6.59235755314445</v>
+        <v>6.6300125396603864</v>
       </c>
       <c r="G8">
         <v>5</v>
       </c>
       <c r="H8">
         <f t="shared" ca="1" si="0"/>
-        <v>6.59235755314445</v>
+        <v>6.6300125396603864</v>
       </c>
       <c r="I8">
         <v>5</v>
       </c>
       <c r="J8">
         <f t="shared" ca="1" si="5"/>
-        <v>6.59235755314445</v>
+        <v>6.6300125396603864</v>
       </c>
       <c r="K8">
         <v>5</v>
       </c>
       <c r="L8">
         <f t="shared" ca="1" si="6"/>
-        <v>6.59235755314445</v>
+        <v>6.6300125396603864</v>
       </c>
       <c r="M8">
         <v>5</v>
       </c>
       <c r="N8">
         <f t="shared" ca="1" si="7"/>
-        <v>6.59235755314445</v>
+        <v>6.6300125396603864</v>
       </c>
       <c r="O8">
         <f t="shared" ca="1" si="1"/>
-        <v>39.554145318866702</v>
+        <v>39.780075237962315</v>
       </c>
     </row>
     <row r="9" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1077,53 +1081,53 @@
       </c>
       <c r="B9" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>1.2662978923109334</v>
+        <v>1.2723842586237939</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
       <c r="D9">
         <f t="shared" ca="1" si="3"/>
-        <v>1.2662978923109334</v>
+        <v>1.2723842586237939</v>
       </c>
       <c r="E9">
         <v>5</v>
       </c>
       <c r="F9">
         <f t="shared" ca="1" si="4"/>
-        <v>6.3314894615546669</v>
+        <v>6.3619212931189697</v>
       </c>
       <c r="G9">
         <v>5</v>
       </c>
       <c r="H9">
         <f t="shared" ca="1" si="0"/>
-        <v>6.3314894615546669</v>
+        <v>6.3619212931189697</v>
       </c>
       <c r="I9">
         <v>5</v>
       </c>
       <c r="J9">
         <f t="shared" ca="1" si="5"/>
-        <v>6.3314894615546669</v>
+        <v>6.3619212931189697</v>
       </c>
       <c r="K9">
         <v>5</v>
       </c>
       <c r="L9">
         <f t="shared" ca="1" si="6"/>
-        <v>6.3314894615546669</v>
+        <v>6.3619212931189697</v>
       </c>
       <c r="M9">
         <v>5</v>
       </c>
       <c r="N9">
         <f t="shared" ca="1" si="7"/>
-        <v>6.3314894615546669</v>
+        <v>6.3619212931189697</v>
       </c>
       <c r="O9">
         <f t="shared" ca="1" si="1"/>
-        <v>32.923745200084269</v>
+        <v>33.081990724218642</v>
       </c>
     </row>
     <row r="10" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1132,53 +1136,53 @@
       </c>
       <c r="B10" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>1.31847151062889</v>
+        <v>1.3260025079320772</v>
       </c>
       <c r="C10">
         <v>5</v>
       </c>
       <c r="D10">
         <f t="shared" ca="1" si="3"/>
-        <v>6.59235755314445</v>
+        <v>6.6300125396603864</v>
       </c>
       <c r="E10">
         <v>5</v>
       </c>
       <c r="F10">
         <f t="shared" ca="1" si="4"/>
-        <v>6.59235755314445</v>
+        <v>6.6300125396603864</v>
       </c>
       <c r="G10">
         <v>5</v>
       </c>
       <c r="H10">
         <f t="shared" ca="1" si="0"/>
-        <v>6.59235755314445</v>
+        <v>6.6300125396603864</v>
       </c>
       <c r="I10">
         <v>5</v>
       </c>
       <c r="J10">
         <f t="shared" ca="1" si="5"/>
-        <v>6.59235755314445</v>
+        <v>6.6300125396603864</v>
       </c>
       <c r="K10">
         <v>5</v>
       </c>
       <c r="L10">
         <f t="shared" ca="1" si="6"/>
-        <v>6.59235755314445</v>
+        <v>6.6300125396603864</v>
       </c>
       <c r="M10">
         <v>5</v>
       </c>
       <c r="N10">
         <f t="shared" ca="1" si="7"/>
-        <v>6.59235755314445</v>
+        <v>6.6300125396603864</v>
       </c>
       <c r="O10">
         <f t="shared" ca="1" si="1"/>
-        <v>39.554145318866702</v>
+        <v>39.780075237962315</v>
       </c>
     </row>
     <row r="11" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1187,53 +1191,53 @@
       </c>
       <c r="B11" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>1.31847151062889</v>
+        <v>1.3260025079320772</v>
       </c>
       <c r="C11">
         <v>5</v>
       </c>
       <c r="D11">
         <f t="shared" ca="1" si="3"/>
-        <v>6.59235755314445</v>
+        <v>6.6300125396603864</v>
       </c>
       <c r="E11">
         <v>5</v>
       </c>
       <c r="F11">
         <f t="shared" ca="1" si="4"/>
-        <v>6.59235755314445</v>
+        <v>6.6300125396603864</v>
       </c>
       <c r="G11">
         <v>5</v>
       </c>
       <c r="H11">
         <f t="shared" ca="1" si="0"/>
-        <v>6.59235755314445</v>
+        <v>6.6300125396603864</v>
       </c>
       <c r="I11">
         <v>5</v>
       </c>
       <c r="J11">
         <f t="shared" ca="1" si="5"/>
-        <v>6.59235755314445</v>
+        <v>6.6300125396603864</v>
       </c>
       <c r="K11">
         <v>5</v>
       </c>
       <c r="L11">
         <f t="shared" ca="1" si="6"/>
-        <v>6.59235755314445</v>
+        <v>6.6300125396603864</v>
       </c>
       <c r="M11">
         <v>5</v>
       </c>
       <c r="N11">
         <f t="shared" ca="1" si="7"/>
-        <v>6.59235755314445</v>
+        <v>6.6300125396603864</v>
       </c>
       <c r="O11">
         <f t="shared" ca="1" si="1"/>
-        <v>39.554145318866702</v>
+        <v>39.780075237962315</v>
       </c>
     </row>
     <row r="12" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1242,53 +1246,53 @@
       </c>
       <c r="B12" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>1.31847151062889</v>
+        <v>1.3260025079320772</v>
       </c>
       <c r="C12">
         <v>5</v>
       </c>
       <c r="D12">
         <f t="shared" ca="1" si="3"/>
-        <v>6.59235755314445</v>
+        <v>6.6300125396603864</v>
       </c>
       <c r="E12">
         <v>5</v>
       </c>
       <c r="F12">
         <f t="shared" ca="1" si="4"/>
-        <v>6.59235755314445</v>
+        <v>6.6300125396603864</v>
       </c>
       <c r="G12">
         <v>5</v>
       </c>
       <c r="H12">
         <f t="shared" ca="1" si="0"/>
-        <v>6.59235755314445</v>
+        <v>6.6300125396603864</v>
       </c>
       <c r="I12">
         <v>5</v>
       </c>
       <c r="J12">
         <f t="shared" ca="1" si="5"/>
-        <v>6.59235755314445</v>
+        <v>6.6300125396603864</v>
       </c>
       <c r="K12">
         <v>5</v>
       </c>
       <c r="L12">
         <f t="shared" ca="1" si="6"/>
-        <v>6.59235755314445</v>
+        <v>6.6300125396603864</v>
       </c>
       <c r="M12">
         <v>5</v>
       </c>
       <c r="N12">
         <f t="shared" ca="1" si="7"/>
-        <v>6.59235755314445</v>
+        <v>6.6300125396603864</v>
       </c>
       <c r="O12">
         <f t="shared" ca="1" si="1"/>
-        <v>39.554145318866702</v>
+        <v>39.780075237962315</v>
       </c>
     </row>
     <row r="13" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1297,7 +1301,7 @@
       </c>
       <c r="B13" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>1.2538078041894074</v>
+        <v>1.2595584210043855</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -1311,39 +1315,39 @@
       </c>
       <c r="F13">
         <f t="shared" ca="1" si="4"/>
-        <v>6.2690390209470372</v>
+        <v>6.2977921050219274</v>
       </c>
       <c r="G13">
         <v>5</v>
       </c>
       <c r="H13">
         <f t="shared" ca="1" si="0"/>
-        <v>6.2690390209470372</v>
+        <v>6.2977921050219274</v>
       </c>
       <c r="I13">
         <v>5</v>
       </c>
       <c r="J13">
         <f t="shared" ca="1" si="5"/>
-        <v>6.2690390209470372</v>
+        <v>6.2977921050219274</v>
       </c>
       <c r="K13">
         <v>5</v>
       </c>
       <c r="L13">
         <f t="shared" ca="1" si="6"/>
-        <v>6.2690390209470372</v>
+        <v>6.2977921050219274</v>
       </c>
       <c r="M13">
         <v>5</v>
       </c>
       <c r="N13">
         <f t="shared" ca="1" si="7"/>
-        <v>6.2690390209470372</v>
+        <v>6.2977921050219274</v>
       </c>
       <c r="O13">
         <f t="shared" ca="1" si="1"/>
-        <v>31.345195104735186</v>
+        <v>31.488960525109636</v>
       </c>
     </row>
     <row r="14" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1352,53 +1356,53 @@
       </c>
       <c r="B14" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>1.31847151062889</v>
+        <v>1.3260025079320772</v>
       </c>
       <c r="C14">
         <v>5</v>
       </c>
       <c r="D14">
         <f t="shared" ca="1" si="3"/>
-        <v>6.59235755314445</v>
+        <v>6.6300125396603864</v>
       </c>
       <c r="E14">
         <v>5</v>
       </c>
       <c r="F14">
         <f t="shared" ca="1" si="4"/>
-        <v>6.59235755314445</v>
+        <v>6.6300125396603864</v>
       </c>
       <c r="G14">
         <v>5</v>
       </c>
       <c r="H14">
         <f t="shared" ca="1" si="0"/>
-        <v>6.59235755314445</v>
+        <v>6.6300125396603864</v>
       </c>
       <c r="I14">
         <v>5</v>
       </c>
       <c r="J14">
         <f t="shared" ca="1" si="5"/>
-        <v>6.59235755314445</v>
+        <v>6.6300125396603864</v>
       </c>
       <c r="K14">
         <v>5</v>
       </c>
       <c r="L14">
         <f t="shared" ca="1" si="6"/>
-        <v>6.59235755314445</v>
+        <v>6.6300125396603864</v>
       </c>
       <c r="M14">
         <v>5</v>
       </c>
       <c r="N14">
         <f t="shared" ca="1" si="7"/>
-        <v>6.59235755314445</v>
+        <v>6.6300125396603864</v>
       </c>
       <c r="O14">
         <f t="shared" ca="1" si="1"/>
-        <v>39.554145318866702</v>
+        <v>39.780075237962315</v>
       </c>
     </row>
     <row r="15" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1407,53 +1411,53 @@
       </c>
       <c r="B15" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>1.31847151062889</v>
+        <v>1.3260025079320772</v>
       </c>
       <c r="C15">
         <v>5</v>
       </c>
       <c r="D15">
         <f t="shared" ca="1" si="3"/>
-        <v>6.59235755314445</v>
+        <v>6.6300125396603864</v>
       </c>
       <c r="E15">
         <v>5</v>
       </c>
       <c r="F15">
         <f t="shared" ca="1" si="4"/>
-        <v>6.59235755314445</v>
+        <v>6.6300125396603864</v>
       </c>
       <c r="G15">
         <v>5</v>
       </c>
       <c r="H15">
         <f t="shared" ca="1" si="0"/>
-        <v>6.59235755314445</v>
+        <v>6.6300125396603864</v>
       </c>
       <c r="I15">
         <v>5</v>
       </c>
       <c r="J15">
         <f t="shared" ca="1" si="5"/>
-        <v>6.59235755314445</v>
+        <v>6.6300125396603864</v>
       </c>
       <c r="K15">
         <v>5</v>
       </c>
       <c r="L15">
         <f t="shared" ca="1" si="6"/>
-        <v>6.59235755314445</v>
+        <v>6.6300125396603864</v>
       </c>
       <c r="M15">
         <v>5</v>
       </c>
       <c r="N15">
         <f t="shared" ca="1" si="7"/>
-        <v>6.59235755314445</v>
+        <v>6.6300125396603864</v>
       </c>
       <c r="O15">
         <f t="shared" ca="1" si="1"/>
-        <v>39.554145318866702</v>
+        <v>39.780075237962315</v>
       </c>
     </row>
     <row r="16" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1462,53 +1466,53 @@
       </c>
       <c r="B16" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>1.31847151062889</v>
+        <v>1.3260025079320772</v>
       </c>
       <c r="C16">
         <v>5</v>
       </c>
       <c r="D16">
         <f t="shared" ca="1" si="3"/>
-        <v>6.59235755314445</v>
+        <v>6.6300125396603864</v>
       </c>
       <c r="E16">
         <v>5</v>
       </c>
       <c r="F16">
         <f t="shared" ca="1" si="4"/>
-        <v>6.59235755314445</v>
+        <v>6.6300125396603864</v>
       </c>
       <c r="G16">
         <v>5</v>
       </c>
       <c r="H16">
         <f t="shared" ca="1" si="0"/>
-        <v>6.59235755314445</v>
+        <v>6.6300125396603864</v>
       </c>
       <c r="I16">
         <v>5</v>
       </c>
       <c r="J16">
         <f t="shared" ca="1" si="5"/>
-        <v>6.59235755314445</v>
+        <v>6.6300125396603864</v>
       </c>
       <c r="K16">
         <v>5</v>
       </c>
       <c r="L16">
         <f t="shared" ca="1" si="6"/>
-        <v>6.59235755314445</v>
+        <v>6.6300125396603864</v>
       </c>
       <c r="M16">
         <v>5</v>
       </c>
       <c r="N16">
         <f t="shared" ca="1" si="7"/>
-        <v>6.59235755314445</v>
+        <v>6.6300125396603864</v>
       </c>
       <c r="O16">
         <f t="shared" ca="1" si="1"/>
-        <v>39.554145318866702</v>
+        <v>39.780075237962315</v>
       </c>
     </row>
     <row r="17" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1517,53 +1521,53 @@
       </c>
       <c r="B17" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>1.31847151062889</v>
+        <v>1.3260025079320772</v>
       </c>
       <c r="C17">
         <v>5</v>
       </c>
       <c r="D17">
         <f t="shared" ca="1" si="3"/>
-        <v>6.59235755314445</v>
+        <v>6.6300125396603864</v>
       </c>
       <c r="E17">
         <v>5</v>
       </c>
       <c r="F17">
         <f t="shared" ca="1" si="4"/>
-        <v>6.59235755314445</v>
+        <v>6.6300125396603864</v>
       </c>
       <c r="G17">
         <v>5</v>
       </c>
       <c r="H17">
         <f t="shared" ca="1" si="0"/>
-        <v>6.59235755314445</v>
+        <v>6.6300125396603864</v>
       </c>
       <c r="I17">
         <v>5</v>
       </c>
       <c r="J17">
         <f t="shared" ca="1" si="5"/>
-        <v>6.59235755314445</v>
+        <v>6.6300125396603864</v>
       </c>
       <c r="K17">
         <v>5</v>
       </c>
       <c r="L17">
         <f t="shared" ca="1" si="6"/>
-        <v>6.59235755314445</v>
+        <v>6.6300125396603864</v>
       </c>
       <c r="M17">
         <v>5</v>
       </c>
       <c r="N17">
         <f t="shared" ca="1" si="7"/>
-        <v>6.59235755314445</v>
+        <v>6.6300125396603864</v>
       </c>
       <c r="O17">
         <f t="shared" ca="1" si="1"/>
-        <v>39.554145318866702</v>
+        <v>39.780075237962315</v>
       </c>
     </row>
     <row r="18" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1572,53 +1576,53 @@
       </c>
       <c r="B18" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>1.31847151062889</v>
+        <v>1.3260025079320772</v>
       </c>
       <c r="C18">
         <v>5</v>
       </c>
       <c r="D18">
         <f t="shared" ca="1" si="3"/>
-        <v>6.59235755314445</v>
+        <v>6.6300125396603864</v>
       </c>
       <c r="E18">
         <v>5</v>
       </c>
       <c r="F18">
         <f t="shared" ca="1" si="4"/>
-        <v>6.59235755314445</v>
+        <v>6.6300125396603864</v>
       </c>
       <c r="G18">
         <v>5</v>
       </c>
       <c r="H18">
         <f t="shared" ca="1" si="0"/>
-        <v>6.59235755314445</v>
+        <v>6.6300125396603864</v>
       </c>
       <c r="I18">
         <v>5</v>
       </c>
       <c r="J18">
         <f t="shared" ca="1" si="5"/>
-        <v>6.59235755314445</v>
+        <v>6.6300125396603864</v>
       </c>
       <c r="K18">
         <v>5</v>
       </c>
       <c r="L18">
         <f t="shared" ca="1" si="6"/>
-        <v>6.59235755314445</v>
+        <v>6.6300125396603864</v>
       </c>
       <c r="M18">
         <v>5</v>
       </c>
       <c r="N18">
         <f t="shared" ca="1" si="7"/>
-        <v>6.59235755314445</v>
+        <v>6.6300125396603864</v>
       </c>
       <c r="O18">
         <f t="shared" ca="1" si="1"/>
-        <v>39.554145318866702</v>
+        <v>39.780075237962315</v>
       </c>
     </row>
     <row r="19" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1627,53 +1631,53 @@
       </c>
       <c r="B19" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>1.31847151062889</v>
+        <v>1.3260025079320772</v>
       </c>
       <c r="C19">
         <v>5</v>
       </c>
       <c r="D19">
         <f t="shared" ca="1" si="3"/>
-        <v>6.59235755314445</v>
+        <v>6.6300125396603864</v>
       </c>
       <c r="E19">
         <v>5</v>
       </c>
       <c r="F19">
         <f t="shared" ca="1" si="4"/>
-        <v>6.59235755314445</v>
+        <v>6.6300125396603864</v>
       </c>
       <c r="G19">
         <v>5</v>
       </c>
       <c r="H19">
         <f t="shared" ca="1" si="0"/>
-        <v>6.59235755314445</v>
+        <v>6.6300125396603864</v>
       </c>
       <c r="I19">
         <v>5</v>
       </c>
       <c r="J19">
         <f t="shared" ca="1" si="5"/>
-        <v>6.59235755314445</v>
+        <v>6.6300125396603864</v>
       </c>
       <c r="K19">
         <v>5</v>
       </c>
       <c r="L19">
         <f t="shared" ca="1" si="6"/>
-        <v>6.59235755314445</v>
+        <v>6.6300125396603864</v>
       </c>
       <c r="M19">
         <v>5</v>
       </c>
       <c r="N19">
         <f t="shared" ca="1" si="7"/>
-        <v>6.59235755314445</v>
+        <v>6.6300125396603864</v>
       </c>
       <c r="O19">
         <f t="shared" ca="1" si="1"/>
-        <v>39.554145318866702</v>
+        <v>39.780075237962315</v>
       </c>
     </row>
     <row r="20" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1682,80 +1686,80 @@
       </c>
       <c r="B20" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>1.31847151062889</v>
+        <v>1.3260025079320772</v>
       </c>
       <c r="C20">
         <v>5</v>
       </c>
       <c r="D20">
         <f t="shared" ca="1" si="3"/>
-        <v>6.59235755314445</v>
+        <v>6.6300125396603864</v>
       </c>
       <c r="E20">
         <v>5</v>
       </c>
       <c r="F20">
         <f t="shared" ca="1" si="4"/>
-        <v>6.59235755314445</v>
+        <v>6.6300125396603864</v>
       </c>
       <c r="G20">
         <v>5</v>
       </c>
       <c r="H20">
         <f t="shared" ca="1" si="0"/>
-        <v>6.59235755314445</v>
+        <v>6.6300125396603864</v>
       </c>
       <c r="I20">
         <v>5</v>
       </c>
       <c r="J20">
         <f t="shared" ca="1" si="5"/>
-        <v>6.59235755314445</v>
+        <v>6.6300125396603864</v>
       </c>
       <c r="K20">
         <v>5</v>
       </c>
       <c r="L20">
         <f t="shared" ca="1" si="6"/>
-        <v>6.59235755314445</v>
+        <v>6.6300125396603864</v>
       </c>
       <c r="M20">
         <v>5</v>
       </c>
       <c r="N20">
         <f t="shared" ca="1" si="7"/>
-        <v>6.59235755314445</v>
+        <v>6.6300125396603864</v>
       </c>
       <c r="O20">
         <f t="shared" ca="1" si="1"/>
-        <v>39.554145318866702</v>
+        <v>39.780075237962315</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B21" s="2"/>
       <c r="D21">
         <f ca="1">SUM(D3:D20)</f>
-        <v>106.74401874262216</v>
+        <v>94.092559813869187</v>
       </c>
       <c r="F21">
         <f ca="1">SUM(F3:F20)</f>
-        <v>118.07824933281293</v>
+        <v>118.07547242511831</v>
       </c>
       <c r="H21">
         <f ca="1">SUM(H3:H20)</f>
-        <v>118.07824933281293</v>
+        <v>118.07547242511831</v>
       </c>
       <c r="J21">
         <f ca="1">SUM(J3:J20)</f>
-        <v>118.07824933281293</v>
+        <v>118.07547242511831</v>
       </c>
       <c r="L21">
         <f ca="1">SUM(L3:L20)</f>
-        <v>118.07824933281293</v>
+        <v>118.07547242511831</v>
       </c>
       <c r="N21">
         <f ca="1">SUM(N3:N20)</f>
-        <v>118.07824933281293</v>
+        <v>118.07547242511831</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
@@ -1766,7 +1770,7 @@
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B26" cm="1">
         <f t="array" aca="1" ref="B26" ca="1">SUM(D3:D20+F3:F20+H3:H20+J3:J20+L3:L20+N3:N20)</f>
-        <v>697.13526540668681</v>
+        <v>684.46992193946096</v>
       </c>
     </row>
   </sheetData>

</xml_diff>